<commit_message>
chỉnh sửa giao diện
</commit_message>
<xml_diff>
--- a/timetabling_GA/results/PS_CT002_HK1/LichHocKy_PS_CT002_HK1.xlsx
+++ b/timetabling_GA/results/PS_CT002_HK1/LichHocKy_PS_CT002_HK1.xlsx
@@ -84,14 +84,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00BDD7EE"/>
-        <bgColor rgb="00BDD7EE"/>
+        <fgColor rgb="00FFCCCB"/>
+        <bgColor rgb="00FFCCCB"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFCCCB"/>
-        <bgColor rgb="00FFCCCB"/>
+        <fgColor rgb="00BDD7EE"/>
+        <bgColor rgb="00BDD7EE"/>
       </patternFill>
     </fill>
   </fills>
@@ -515,6 +515,340 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="8" max="8"/>
+    <col width="25" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>CANTHO UNIVERSITY SOFTWARE CENTER</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>TRUNG TÂM PHẦN MỀM ĐẠI HỌC CẦN THƠ</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Khu 3, Đại học Cần Thơ - 01 Lý Tự Trọng, TP Cần Thơ - Tel: 0292.3731072 &amp; Fax: 0292.3731071 - Email: cusc@ctu.edu.vn</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>WEEK 1 TIMETABLE (11/08/2025 - 17/08/2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="40" customHeight="1">
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>Time Slot</t>
+        </is>
+      </c>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>Class</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>Students</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>Monday
+11/08</t>
+        </is>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>Tuesday
+12/08</t>
+        </is>
+      </c>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>Wednesday
+13/08</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>Thursday
+14/08</t>
+        </is>
+      </c>
+      <c r="H7" s="5" t="inlineStr">
+        <is>
+          <t>Friday
+15/08</t>
+        </is>
+      </c>
+      <c r="I7" s="5" t="inlineStr">
+        <is>
+          <t>Saturday
+16/08</t>
+        </is>
+      </c>
+      <c r="J7" s="5" t="inlineStr">
+        <is>
+          <t>Sunday
+17/08</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="60" customHeight="1">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="7" t="inlineStr"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>MH001
+(Practice)
+Room: TH1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I8" s="8" t="inlineStr">
+        <is>
+          <t>MH002
+(Practice)
+Room: TH1
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: A102
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="I9" s="9" t="inlineStr">
+        <is>
+          <t>MH012
+(Theory)
+Room: LT2
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="J9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="I10" s="8" t="inlineStr">
+        <is>
+          <t>MH012
+(Practice)
+Room: TH3
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="7" t="inlineStr"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="7" t="inlineStr"/>
+      <c r="I11" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: A101
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="7" t="inlineStr"/>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>MH001
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I12" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Practice)
+Room: TH3
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I13" s="9" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: A101
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -559,7 +893,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 1 TIMETABLE (11/08/2025 - 17/08/2025)</t>
+          <t>WEEK 10 TIMETABLE (13/10/2025 - 19/10/2025)</t>
         </is>
       </c>
     </row>
@@ -582,43 +916,43 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-11/08</t>
+13/10</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-12/08</t>
+14/10</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-13/08</t>
+15/10</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-14/08</t>
+16/10</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-15/08</t>
+17/10</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-16/08</t>
+18/10</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-17/08</t>
+19/10</t>
         </is>
       </c>
     </row>
@@ -639,11 +973,11 @@
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
+      <c r="G8" s="9" t="inlineStr">
         <is>
           <t>MH001
 (Theory)
-Room: LT3
+Room: A101
 Lecturer: GV001</t>
         </is>
       </c>
@@ -654,7 +988,7 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -665,31 +999,17 @@
       <c r="C9" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>MH016
-(Practice)
-Room: TH1
-Lecturer: GV006</t>
-        </is>
-      </c>
+      <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="9" t="inlineStr">
-        <is>
-          <t>MH001
-(Practice)
-Room: TH3
-Lecturer: GV001</t>
-        </is>
-      </c>
+      <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH015
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
+      <c r="I9" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
         </is>
       </c>
       <c r="J9" s="7" t="inlineStr"/>
@@ -697,7 +1017,7 @@
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
@@ -709,31 +1029,24 @@
         <v>30</v>
       </c>
       <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="9" t="inlineStr">
-        <is>
-          <t>MH002
-(Practice)
-Room: TH3
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="9" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: A102
 Lecturer: GV008</t>
         </is>
       </c>
-      <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
       <c r="H10" s="7" t="inlineStr"/>
-      <c r="I10" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT3
-Lecturer: GV008</t>
-        </is>
-      </c>
+      <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -744,30 +1057,16 @@
       <c r="C11" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>MH009
-(Practice)
-Room: TH3
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="9" t="inlineStr">
-        <is>
-          <t>MH015
-(Practice)
-Room: TH2
-Lecturer: GV008</t>
-        </is>
-      </c>
+      <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH016
-(Theory)
-Room: LT2
-Lecturer: GV006</t>
+      <c r="H11" s="9" t="inlineStr">
+        <is>
+          <t>MH012
+(Theory)
+Room: LT1
+Lecturer: GV005</t>
         </is>
       </c>
       <c r="I11" s="7" t="inlineStr"/>
@@ -776,7 +1075,7 @@
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="B12" s="7" t="inlineStr">
@@ -788,32 +1087,18 @@
         <v>30</v>
       </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="8" t="inlineStr">
-        <is>
-          <t>MH009
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="E12" s="7" t="inlineStr"/>
       <c r="F12" s="7" t="inlineStr"/>
       <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT2
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="I12" s="8" t="inlineStr">
+      <c r="H12" s="9" t="inlineStr">
         <is>
           <t>MH002
 (Theory)
 Room: LT1
-Lecturer: GV001</t>
-        </is>
-      </c>
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="I12" s="7" t="inlineStr"/>
       <c r="J12" s="7" t="inlineStr"/>
     </row>
     <row r="13"/>
@@ -828,13 +1113,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -878,7 +1163,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 10 TIMETABLE (13/10/2025 - 19/10/2025)</t>
+          <t>WEEK 11 TIMETABLE (20/10/2025 - 26/10/2025)</t>
         </is>
       </c>
     </row>
@@ -901,43 +1186,43 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-13/10</t>
+20/10</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-14/10</t>
+21/10</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-15/10</t>
+22/10</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-16/10</t>
+23/10</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-17/10</t>
+24/10</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-18/10</t>
+25/10</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-19/10</t>
+26/10</t>
         </is>
       </c>
     </row>
@@ -958,11 +1243,11 @@
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
+      <c r="G8" s="9" t="inlineStr">
         <is>
           <t>MH001
 (Theory)
-Room: LT3
+Room: A101
 Lecturer: GV001</t>
         </is>
       </c>
@@ -973,7 +1258,7 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -989,12 +1274,12 @@
       <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH015
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
+      <c r="I9" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
         </is>
       </c>
       <c r="J9" s="7" t="inlineStr"/>
@@ -1016,15 +1301,15 @@
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="8" t="inlineStr">
-        <is>
-          <t>MH016
-(Theory)
-Room: LT2
-Lecturer: GV006</t>
-        </is>
-      </c>
+      <c r="G10" s="9" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: A102
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
@@ -1043,35 +1328,50 @@
         <v>30</v>
       </c>
       <c r="D11" s="7" t="inlineStr"/>
-      <c r="E11" s="8" t="inlineStr">
-        <is>
-          <t>MH009
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="E11" s="7" t="inlineStr"/>
       <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
+      <c r="H11" s="9" t="inlineStr">
+        <is>
+          <t>MH012
+(Theory)
+Room: LT1
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="7" t="inlineStr"/>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT1
 Lecturer: GV008</t>
         </is>
       </c>
-      <c r="I11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT1
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="J11" s="7" t="inlineStr"/>
-    </row>
-    <row r="12"/>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
@@ -1083,13 +1383,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1133,7 +1433,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 11 TIMETABLE (20/10/2025 - 26/10/2025)</t>
+          <t>WEEK 12 TIMETABLE (27/10/2025 - 02/11/2025)</t>
         </is>
       </c>
     </row>
@@ -1156,43 +1456,43 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-20/10</t>
+27/10</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-21/10</t>
+28/10</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-22/10</t>
+29/10</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-23/10</t>
+30/10</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-24/10</t>
+31/10</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-25/10</t>
+01/11</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-26/10</t>
+02/11</t>
         </is>
       </c>
     </row>
@@ -1213,11 +1513,11 @@
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
+      <c r="G8" s="9" t="inlineStr">
         <is>
           <t>MH001
 (Theory)
-Room: LT3
+Room: A101
 Lecturer: GV001</t>
         </is>
       </c>
@@ -1228,7 +1528,7 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1244,12 +1544,12 @@
       <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH015
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
+      <c r="I9" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
         </is>
       </c>
       <c r="J9" s="7" t="inlineStr"/>
@@ -1271,15 +1571,15 @@
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="8" t="inlineStr">
-        <is>
-          <t>MH016
-(Theory)
-Room: LT2
-Lecturer: GV006</t>
-        </is>
-      </c>
+      <c r="G10" s="9" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: A102
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
@@ -1298,35 +1598,50 @@
         <v>30</v>
       </c>
       <c r="D11" s="7" t="inlineStr"/>
-      <c r="E11" s="8" t="inlineStr">
-        <is>
-          <t>MH009
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="E11" s="7" t="inlineStr"/>
       <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
+      <c r="H11" s="9" t="inlineStr">
+        <is>
+          <t>MH012
+(Theory)
+Room: LT1
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="7" t="inlineStr"/>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT1
 Lecturer: GV008</t>
         </is>
       </c>
-      <c r="I11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT1
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="J11" s="7" t="inlineStr"/>
-    </row>
-    <row r="12"/>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
@@ -1338,13 +1653,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1388,7 +1703,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 12 TIMETABLE (27/10/2025 - 02/11/2025)</t>
+          <t>WEEK 13 TIMETABLE (03/11/2025 - 09/11/2025)</t>
         </is>
       </c>
     </row>
@@ -1411,43 +1726,43 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-27/10</t>
+03/11</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-28/10</t>
+04/11</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-29/10</t>
+05/11</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-30/10</t>
+06/11</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-31/10</t>
+07/11</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-01/11</t>
+08/11</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-02/11</t>
+09/11</t>
         </is>
       </c>
     </row>
@@ -1468,11 +1783,11 @@
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
+      <c r="G8" s="9" t="inlineStr">
         <is>
           <t>MH001
 (Theory)
-Room: LT3
+Room: A101
 Lecturer: GV001</t>
         </is>
       </c>
@@ -1483,7 +1798,7 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1499,12 +1814,12 @@
       <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH015
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
+      <c r="I9" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
         </is>
       </c>
       <c r="J9" s="7" t="inlineStr"/>
@@ -1526,15 +1841,15 @@
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="8" t="inlineStr">
-        <is>
-          <t>MH016
-(Theory)
-Room: LT2
-Lecturer: GV006</t>
-        </is>
-      </c>
+      <c r="G10" s="9" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: A102
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
@@ -1553,35 +1868,50 @@
         <v>30</v>
       </c>
       <c r="D11" s="7" t="inlineStr"/>
-      <c r="E11" s="8" t="inlineStr">
-        <is>
-          <t>MH009
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="E11" s="7" t="inlineStr"/>
       <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
+      <c r="H11" s="9" t="inlineStr">
+        <is>
+          <t>MH012
+(Theory)
+Room: LT1
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="7" t="inlineStr"/>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT1
 Lecturer: GV008</t>
         </is>
       </c>
-      <c r="I11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT1
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="J11" s="7" t="inlineStr"/>
-    </row>
-    <row r="12"/>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
@@ -1593,13 +1923,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1643,7 +1973,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 13 TIMETABLE (03/11/2025 - 09/11/2025)</t>
+          <t>WEEK 14 TIMETABLE (10/11/2025 - 16/11/2025)</t>
         </is>
       </c>
     </row>
@@ -1666,43 +1996,43 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-03/11</t>
+10/11</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-04/11</t>
+11/11</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-05/11</t>
+12/11</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-06/11</t>
+13/11</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-07/11</t>
+14/11</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-08/11</t>
+15/11</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-09/11</t>
+16/11</t>
         </is>
       </c>
     </row>
@@ -1723,11 +2053,11 @@
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
+      <c r="G8" s="9" t="inlineStr">
         <is>
           <t>MH001
 (Theory)
-Room: LT3
+Room: A101
 Lecturer: GV001</t>
         </is>
       </c>
@@ -1738,7 +2068,7 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1754,12 +2084,12 @@
       <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH015
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
+      <c r="I9" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
         </is>
       </c>
       <c r="J9" s="7" t="inlineStr"/>
@@ -1781,15 +2111,15 @@
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="8" t="inlineStr">
-        <is>
-          <t>MH016
-(Theory)
-Room: LT2
-Lecturer: GV006</t>
-        </is>
-      </c>
+      <c r="G10" s="9" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: A102
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
@@ -1808,35 +2138,50 @@
         <v>30</v>
       </c>
       <c r="D11" s="7" t="inlineStr"/>
-      <c r="E11" s="8" t="inlineStr">
-        <is>
-          <t>MH009
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="E11" s="7" t="inlineStr"/>
       <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
+      <c r="H11" s="9" t="inlineStr">
+        <is>
+          <t>MH012
+(Theory)
+Room: LT1
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="7" t="inlineStr"/>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT1
 Lecturer: GV008</t>
         </is>
       </c>
-      <c r="I11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT1
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="J11" s="7" t="inlineStr"/>
-    </row>
-    <row r="12"/>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
@@ -1848,13 +2193,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1898,7 +2243,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 14 TIMETABLE (10/11/2025 - 16/11/2025)</t>
+          <t>WEEK 15 TIMETABLE (17/11/2025 - 23/11/2025)</t>
         </is>
       </c>
     </row>
@@ -1921,43 +2266,43 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-10/11</t>
+17/11</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-11/11</t>
+18/11</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-12/11</t>
+19/11</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-13/11</t>
+20/11</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-14/11</t>
+21/11</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-15/11</t>
+22/11</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-16/11</t>
+23/11</t>
         </is>
       </c>
     </row>
@@ -1978,11 +2323,11 @@
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
+      <c r="G8" s="9" t="inlineStr">
         <is>
           <t>MH001
 (Theory)
-Room: LT3
+Room: A101
 Lecturer: GV001</t>
         </is>
       </c>
@@ -1993,7 +2338,7 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2009,12 +2354,12 @@
       <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH015
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
+      <c r="I9" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
         </is>
       </c>
       <c r="J9" s="7" t="inlineStr"/>
@@ -2036,15 +2381,15 @@
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="8" t="inlineStr">
-        <is>
-          <t>MH016
-(Theory)
-Room: LT2
-Lecturer: GV006</t>
-        </is>
-      </c>
+      <c r="G10" s="9" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: A102
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
@@ -2063,290 +2408,50 @@
         <v>30</v>
       </c>
       <c r="D11" s="7" t="inlineStr"/>
-      <c r="E11" s="8" t="inlineStr">
-        <is>
-          <t>MH009
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="E11" s="7" t="inlineStr"/>
       <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
+      <c r="H11" s="9" t="inlineStr">
+        <is>
+          <t>MH012
+(Theory)
+Room: LT1
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="7" t="inlineStr"/>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT1
 Lecturer: GV008</t>
         </is>
       </c>
-      <c r="I11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT1
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="J11" s="7" t="inlineStr"/>
-    </row>
-    <row r="12"/>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A2:J2"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="25" customWidth="1" min="4" max="4"/>
-    <col width="25" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
-    <col width="25" customWidth="1" min="7" max="7"/>
-    <col width="25" customWidth="1" min="8" max="8"/>
-    <col width="25" customWidth="1" min="9" max="9"/>
-    <col width="25" customWidth="1" min="10" max="10"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>CANTHO UNIVERSITY SOFTWARE CENTER</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>TRUNG TÂM PHẦN MỀM ĐẠI HỌC CẦN THƠ</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>Khu 3, Đại học Cần Thơ - 01 Lý Tự Trọng, TP Cần Thơ - Tel: 0292.3731072 &amp; Fax: 0292.3731071 - Email: cusc@ctu.edu.vn</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>WEEK 15 TIMETABLE (17/11/2025 - 23/11/2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="40" customHeight="1">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>Time Slot</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>Class</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>Students</t>
-        </is>
-      </c>
-      <c r="D7" s="5" t="inlineStr">
-        <is>
-          <t>Monday
-17/11</t>
-        </is>
-      </c>
-      <c r="E7" s="5" t="inlineStr">
-        <is>
-          <t>Tuesday
-18/11</t>
-        </is>
-      </c>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>Wednesday
-19/11</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="inlineStr">
-        <is>
-          <t>Thursday
-20/11</t>
-        </is>
-      </c>
-      <c r="H7" s="5" t="inlineStr">
-        <is>
-          <t>Friday
-21/11</t>
-        </is>
-      </c>
-      <c r="I7" s="5" t="inlineStr">
-        <is>
-          <t>Saturday
-22/11</t>
-        </is>
-      </c>
-      <c r="J7" s="5" t="inlineStr">
-        <is>
-          <t>Sunday
-23/11</t>
-        </is>
-      </c>
-    </row>
-    <row r="8" ht="60" customHeight="1">
-      <c r="A8" s="6" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="B8" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C8" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>MH001
-(Theory)
-Room: LT3
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="7" t="inlineStr"/>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>C2</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH015
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="7" t="inlineStr"/>
-      <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="8" t="inlineStr">
-        <is>
-          <t>MH016
-(Theory)
-Room: LT2
-Lecturer: GV006</t>
-        </is>
-      </c>
-      <c r="I10" s="7" t="inlineStr"/>
-      <c r="J10" s="7" t="inlineStr"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="7" t="inlineStr"/>
-      <c r="E11" s="8" t="inlineStr">
-        <is>
-          <t>MH009
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
-      <c r="F11" s="7" t="inlineStr"/>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
-Lecturer: GV008</t>
-        </is>
-      </c>
-      <c r="I11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT1
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="J11" s="7" t="inlineStr"/>
-    </row>
-    <row r="12"/>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
@@ -2488,11 +2593,11 @@
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
+      <c r="G8" s="9" t="inlineStr">
         <is>
           <t>MH001
 (Theory)
-Room: LT3
+Room: A101
 Lecturer: GV001</t>
         </is>
       </c>
@@ -2500,176 +2605,162 @@
       <c r="I8" s="8" t="inlineStr">
         <is>
           <t>MH002
+(Practice)
+Room: TH1
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>MH001
+(Practice)
+Room: TH1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I9" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="J9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="9" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: A102
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="7" t="inlineStr"/>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="7" t="inlineStr"/>
+      <c r="G11" s="9" t="inlineStr">
+        <is>
+          <t>MH002
 (Theory)
 Room: LT2
 Lecturer: GV001</t>
         </is>
       </c>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>C2</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>MH016
-(Practice)
-Room: TH1
-Lecturer: GV006</t>
-        </is>
-      </c>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="9" t="inlineStr">
-        <is>
-          <t>MH001
+      <c r="H11" s="9" t="inlineStr">
+        <is>
+          <t>MH012
+(Theory)
+Room: LT1
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="I11" s="8" t="inlineStr">
+        <is>
+          <t>MH013
 (Practice)
 Room: TH3
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: A101
 Lecturer: GV001</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH015
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="9" t="inlineStr">
-        <is>
-          <t>MH002
-(Practice)
-Room: TH3
-Lecturer: GV008</t>
-        </is>
-      </c>
-      <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT2
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="I10" s="7" t="inlineStr"/>
-      <c r="J10" s="7" t="inlineStr"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>MH009
-(Practice)
-Room: TH3
-Lecturer: GV003</t>
-        </is>
-      </c>
-      <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="9" t="inlineStr">
-        <is>
-          <t>MH015
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="8" t="inlineStr">
+        <is>
+          <t>MH012
 (Practice)
 Room: TH2
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT1
 Lecturer: GV008</t>
         </is>
       </c>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH016
-(Theory)
-Room: LT2
-Lecturer: GV006</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="inlineStr"/>
-      <c r="J11" s="7" t="inlineStr"/>
-    </row>
-    <row r="12" ht="60" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="8" t="inlineStr">
-        <is>
-          <t>MH009
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
-      <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
-Lecturer: GV008</t>
-        </is>
-      </c>
-      <c r="I12" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT1
-Lecturer: GV001</t>
-        </is>
-      </c>
+      <c r="I12" s="7" t="inlineStr"/>
       <c r="J12" s="7" t="inlineStr"/>
     </row>
     <row r="13"/>
@@ -2814,172 +2905,158 @@
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
+      <c r="G8" s="9" t="inlineStr">
         <is>
           <t>MH001
+(Theory)
+Room: A101
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H8" s="7" t="inlineStr"/>
+      <c r="I8" s="8" t="inlineStr">
+        <is>
+          <t>MH002
+(Practice)
+Room: TH1
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t>MH002
 (Theory)
 Room: LT3
 Lecturer: GV001</t>
         </is>
       </c>
-      <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="7" t="inlineStr"/>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>C2</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>MH016
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="7" t="inlineStr"/>
+      <c r="J9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D10" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT2
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH001
 (Practice)
 Room: TH1
-Lecturer: GV006</t>
-        </is>
-      </c>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="9" t="inlineStr">
-        <is>
-          <t>MH001
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I10" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="7" t="inlineStr"/>
+      <c r="G11" s="9" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: A102
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H11" s="7" t="inlineStr"/>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="7" t="inlineStr"/>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>MH012
+(Theory)
+Room: LT1
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="I12" s="8" t="inlineStr">
+        <is>
+          <t>MH013
 (Practice)
 Room: TH3
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH015
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="9" t="inlineStr">
-        <is>
-          <t>MH002
-(Practice)
-Room: TH3
-Lecturer: GV008</t>
-        </is>
-      </c>
-      <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
-      <c r="I10" s="7" t="inlineStr"/>
-      <c r="J10" s="7" t="inlineStr"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>MH009
-(Practice)
-Room: TH3
-Lecturer: GV003</t>
-        </is>
-      </c>
-      <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="9" t="inlineStr">
-        <is>
-          <t>MH015
-(Practice)
-Room: TH2
-Lecturer: GV008</t>
-        </is>
-      </c>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH016
-(Theory)
-Room: LT2
-Lecturer: GV006</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="inlineStr"/>
-      <c r="J11" s="7" t="inlineStr"/>
-    </row>
-    <row r="12" ht="60" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="8" t="inlineStr">
-        <is>
-          <t>MH009
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
-      <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
-Lecturer: GV008</t>
-        </is>
-      </c>
-      <c r="I12" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT2
-Lecturer: GV008</t>
+Lecturer: GV005</t>
         </is>
       </c>
       <c r="J12" s="7" t="inlineStr"/>
@@ -3001,12 +3078,19 @@
       <c r="D13" s="7" t="inlineStr"/>
       <c r="E13" s="7" t="inlineStr"/>
       <c r="F13" s="7" t="inlineStr"/>
-      <c r="G13" s="7" t="inlineStr"/>
-      <c r="H13" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
+      <c r="G13" s="8" t="inlineStr">
+        <is>
+          <t>MH012
+(Practice)
+Room: TH2
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="H13" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT1
 Lecturer: GV008</t>
         </is>
       </c>
@@ -3026,6 +3110,340 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
+    <col width="25" customWidth="1" min="8" max="8"/>
+    <col width="25" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>CANTHO UNIVERSITY SOFTWARE CENTER</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>TRUNG TÂM PHẦN MỀM ĐẠI HỌC CẦN THƠ</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>Khu 3, Đại học Cần Thơ - 01 Lý Tự Trọng, TP Cần Thơ - Tel: 0292.3731072 &amp; Fax: 0292.3731071 - Email: cusc@ctu.edu.vn</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>WEEK 4 TIMETABLE (01/09/2025 - 07/09/2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="40" customHeight="1">
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>Time Slot</t>
+        </is>
+      </c>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>Class</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>Students</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>Monday
+01/09</t>
+        </is>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>Tuesday
+02/09</t>
+        </is>
+      </c>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>Wednesday
+03/09</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr">
+        <is>
+          <t>Thursday
+04/09</t>
+        </is>
+      </c>
+      <c r="H7" s="5" t="inlineStr">
+        <is>
+          <t>Friday
+05/09</t>
+        </is>
+      </c>
+      <c r="I7" s="5" t="inlineStr">
+        <is>
+          <t>Saturday
+06/09</t>
+        </is>
+      </c>
+      <c r="J7" s="5" t="inlineStr">
+        <is>
+          <t>Sunday
+07/09</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="60" customHeight="1">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="9" t="inlineStr">
+        <is>
+          <t>MH001
+(Theory)
+Room: A101
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H8" s="7" t="inlineStr"/>
+      <c r="I8" s="8" t="inlineStr">
+        <is>
+          <t>MH002
+(Practice)
+Room: TH1
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="J8" s="7" t="inlineStr"/>
+    </row>
+    <row r="9" ht="60" customHeight="1">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="7" t="inlineStr"/>
+      <c r="I9" s="9" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT4
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="J9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="7" t="inlineStr"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>MH001
+(Practice)
+Room: TH1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I10" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="7" t="inlineStr"/>
+      <c r="G11" s="9" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: A102
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H11" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: A101
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="7" t="inlineStr"/>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>MH012
+(Theory)
+Room: LT1
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="I12" s="8" t="inlineStr">
+        <is>
+          <t>MH013
+(Practice)
+Room: TH3
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13" ht="60" customHeight="1">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7" t="inlineStr"/>
+      <c r="E13" s="7" t="inlineStr"/>
+      <c r="F13" s="7" t="inlineStr"/>
+      <c r="G13" s="7" t="inlineStr"/>
+      <c r="H13" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT1
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="I13" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="J13" s="7" t="inlineStr"/>
+    </row>
+    <row r="14"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3075,7 +3493,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 4 TIMETABLE (01/09/2025 - 07/09/2025)</t>
+          <t>WEEK 5 TIMETABLE (08/09/2025 - 14/09/2025)</t>
         </is>
       </c>
     </row>
@@ -3098,43 +3516,43 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-01/09</t>
+08/09</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-02/09</t>
+09/09</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-03/09</t>
+10/09</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-04/09</t>
+11/09</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-05/09</t>
+12/09</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-06/09</t>
+13/09</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-07/09</t>
+14/09</t>
         </is>
       </c>
     </row>
@@ -3153,24 +3571,38 @@
         <v>30</v>
       </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="7" t="inlineStr"/>
+      <c r="E8" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT2
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
+      <c r="G8" s="9" t="inlineStr">
         <is>
           <t>MH001
 (Theory)
-Room: LT3
+Room: A101
 Lecturer: GV001</t>
         </is>
       </c>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="7" t="inlineStr"/>
+      <c r="I8" s="8" t="inlineStr">
+        <is>
+          <t>MH002
+(Practice)
+Room: TH1
+Lecturer: GV008</t>
+        </is>
+      </c>
       <c r="J8" s="7" t="inlineStr"/>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -3181,125 +3613,97 @@
       <c r="C9" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>MH016
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>MH001
 (Practice)
 Room: TH1
-Lecturer: GV006</t>
-        </is>
-      </c>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="9" t="inlineStr">
-        <is>
-          <t>MH001
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="I9" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="J9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: A102
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
+      <c r="I10" s="7" t="inlineStr"/>
+      <c r="J10" s="7" t="inlineStr"/>
+    </row>
+    <row r="11" ht="60" customHeight="1">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="inlineStr"/>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="7" t="inlineStr"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="9" t="inlineStr">
+        <is>
+          <t>MH012
+(Theory)
+Room: LT1
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="I11" s="8" t="inlineStr">
+        <is>
+          <t>MH013
 (Practice)
 Room: TH3
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH015
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="9" t="inlineStr">
-        <is>
-          <t>MH002
-(Practice)
-Room: TH3
-Lecturer: GV008</t>
-        </is>
-      </c>
-      <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="8" t="inlineStr">
-        <is>
-          <t>MH016
-(Theory)
-Room: LT1
-Lecturer: GV006</t>
-        </is>
-      </c>
-      <c r="I10" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT3
-Lecturer: GV008</t>
-        </is>
-      </c>
-      <c r="J10" s="7" t="inlineStr"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>MH009
-(Practice)
-Room: TH3
-Lecturer: GV003</t>
-        </is>
-      </c>
-      <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="9" t="inlineStr">
-        <is>
-          <t>MH015
-(Practice)
-Room: TH2
-Lecturer: GV008</t>
-        </is>
-      </c>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT2
-Lecturer: GV008</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="inlineStr"/>
+Lecturer: GV005</t>
+        </is>
+      </c>
       <c r="J11" s="7" t="inlineStr"/>
     </row>
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="B12" s="7" t="inlineStr">
@@ -3311,32 +3715,18 @@
         <v>30</v>
       </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="8" t="inlineStr">
-        <is>
-          <t>MH009
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="E12" s="7" t="inlineStr"/>
       <c r="F12" s="7" t="inlineStr"/>
       <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT1
 Lecturer: GV008</t>
         </is>
       </c>
-      <c r="I12" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT1
-Lecturer: GV001</t>
-        </is>
-      </c>
+      <c r="I12" s="7" t="inlineStr"/>
       <c r="J12" s="7" t="inlineStr"/>
     </row>
     <row r="13"/>
@@ -3351,13 +3741,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3401,7 +3791,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 5 TIMETABLE (08/09/2025 - 14/09/2025)</t>
+          <t>WEEK 6 TIMETABLE (15/09/2025 - 21/09/2025)</t>
         </is>
       </c>
     </row>
@@ -3424,43 +3814,43 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-08/09</t>
+15/09</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-09/09</t>
+16/09</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-10/09</t>
+17/09</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-11/09</t>
+18/09</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-12/09</t>
+19/09</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-13/09</t>
+20/09</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-14/09</t>
+21/09</t>
         </is>
       </c>
     </row>
@@ -3481,22 +3871,29 @@
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
+      <c r="G8" s="9" t="inlineStr">
         <is>
           <t>MH001
 (Theory)
-Room: LT3
+Room: A101
 Lecturer: GV001</t>
         </is>
       </c>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="7" t="inlineStr"/>
+      <c r="I8" s="8" t="inlineStr">
+        <is>
+          <t>MH002
+(Practice)
+Room: TH1
+Lecturer: GV008</t>
+        </is>
+      </c>
       <c r="J8" s="7" t="inlineStr"/>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -3507,31 +3904,24 @@
       <c r="C9" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t>MH016
+      <c r="D9" s="7" t="inlineStr"/>
+      <c r="E9" s="7" t="inlineStr"/>
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>MH001
 (Practice)
 Room: TH1
-Lecturer: GV006</t>
-        </is>
-      </c>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="9" t="inlineStr">
-        <is>
-          <t>MH001
-(Practice)
-Room: TH3
 Lecturer: GV001</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH015
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
+      <c r="I9" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
         </is>
       </c>
       <c r="J9" s="7" t="inlineStr"/>
@@ -3539,7 +3929,7 @@
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
@@ -3554,21 +3944,35 @@
       <c r="E10" s="9" t="inlineStr">
         <is>
           <t>MH002
-(Practice)
-Room: TH3
+(Theory)
+Room: LT1
 Lecturer: GV008</t>
         </is>
       </c>
       <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="G10" s="9" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: A102
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H10" s="9" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: LT4
+Lecturer: GV008</t>
+        </is>
+      </c>
       <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -3580,32 +3984,6 @@
         <v>30</v>
       </c>
       <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>MH009
-(Practice)
-Room: TH3
-Lecturer: GV003</t>
-        </is>
-      </c>
-      <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="9" t="inlineStr">
-        <is>
-          <t>MH015
-(Practice)
-Room: TH2
-Lecturer: GV008</t>
-        </is>
-      </c>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH016
-(Theory)
-Room: LT2
-Lecturer: GV006</t>
-        </is>
-      </c>
-      <c r="I11" s="8" t="inlineStr">
         <is>
           <t>MH002
 (Theory)
@@ -3613,12 +3991,24 @@
 Lecturer: GV008</t>
         </is>
       </c>
+      <c r="E11" s="7" t="inlineStr"/>
+      <c r="F11" s="7" t="inlineStr"/>
+      <c r="G11" s="7" t="inlineStr"/>
+      <c r="H11" s="9" t="inlineStr">
+        <is>
+          <t>MH012
+(Theory)
+Room: LT1
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
       <c r="J11" s="7" t="inlineStr"/>
     </row>
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="B12" s="7" t="inlineStr">
@@ -3630,64 +4020,21 @@
         <v>30</v>
       </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="8" t="inlineStr">
-        <is>
-          <t>MH009
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="E12" s="7" t="inlineStr"/>
       <c r="F12" s="7" t="inlineStr"/>
       <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT1
 Lecturer: GV008</t>
         </is>
       </c>
-      <c r="I12" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT1
-Lecturer: GV001</t>
-        </is>
-      </c>
+      <c r="I12" s="7" t="inlineStr"/>
       <c r="J12" s="7" t="inlineStr"/>
     </row>
-    <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B13" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D13" s="7" t="inlineStr"/>
-      <c r="E13" s="7" t="inlineStr"/>
-      <c r="F13" s="7" t="inlineStr"/>
-      <c r="G13" s="7" t="inlineStr"/>
-      <c r="H13" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT3
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="I13" s="7" t="inlineStr"/>
-      <c r="J13" s="7" t="inlineStr"/>
-    </row>
-    <row r="14"/>
+    <row r="13"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
@@ -3699,13 +4046,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3749,7 +4096,7 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>WEEK 6 TIMETABLE (15/09/2025 - 21/09/2025)</t>
+          <t>WEEK 7 TIMETABLE (22/09/2025 - 28/09/2025)</t>
         </is>
       </c>
     </row>
@@ -3772,43 +4119,43 @@
       <c r="D7" s="5" t="inlineStr">
         <is>
           <t>Monday
-15/09</t>
+22/09</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
           <t>Tuesday
-16/09</t>
+23/09</t>
         </is>
       </c>
       <c r="F7" s="5" t="inlineStr">
         <is>
           <t>Wednesday
-17/09</t>
+24/09</t>
         </is>
       </c>
       <c r="G7" s="5" t="inlineStr">
         <is>
           <t>Thursday
-18/09</t>
+25/09</t>
         </is>
       </c>
       <c r="H7" s="5" t="inlineStr">
         <is>
           <t>Friday
-19/09</t>
+26/09</t>
         </is>
       </c>
       <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Saturday
-20/09</t>
+27/09</t>
         </is>
       </c>
       <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Sunday
-21/09</t>
+28/09</t>
         </is>
       </c>
     </row>
@@ -3829,11 +4176,11 @@
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
+      <c r="G8" s="9" t="inlineStr">
         <is>
           <t>MH001
 (Theory)
-Room: LT3
+Room: A101
 Lecturer: GV001</t>
         </is>
       </c>
@@ -3841,8 +4188,8 @@
       <c r="I8" s="8" t="inlineStr">
         <is>
           <t>MH002
-(Theory)
-Room: LT2
+(Practice)
+Room: TH1
 Lecturer: GV008</t>
         </is>
       </c>
@@ -3851,7 +4198,7 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -3864,22 +4211,22 @@
       </c>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="9" t="inlineStr">
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
         <is>
           <t>MH001
 (Practice)
-Room: TH3
+Room: TH1
 Lecturer: GV001</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH015
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
+      <c r="I9" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
         </is>
       </c>
       <c r="J9" s="7" t="inlineStr"/>
@@ -3887,7 +4234,7 @@
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
@@ -3899,24 +4246,31 @@
         <v>30</v>
       </c>
       <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="9" t="inlineStr">
-        <is>
-          <t>MH002
-(Practice)
-Room: TH3
-Lecturer: GV008</t>
-        </is>
-      </c>
+      <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
+      <c r="G10" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT1
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="H10" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: A102
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -3927,23 +4281,16 @@
       <c r="C11" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>MH009
-(Practice)
-Room: TH3
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
       <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH016
-(Theory)
-Room: LT2
-Lecturer: GV006</t>
+      <c r="H11" s="9" t="inlineStr">
+        <is>
+          <t>MH012
+(Theory)
+Room: LT1
+Lecturer: GV005</t>
         </is>
       </c>
       <c r="I11" s="7" t="inlineStr"/>
@@ -3952,7 +4299,7 @@
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="B12" s="7" t="inlineStr">
@@ -3964,391 +4311,21 @@
         <v>30</v>
       </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="8" t="inlineStr">
-        <is>
-          <t>MH009
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="E12" s="7" t="inlineStr"/>
       <c r="F12" s="7" t="inlineStr"/>
       <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT1
 Lecturer: GV008</t>
         </is>
       </c>
-      <c r="I12" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT1
-Lecturer: GV001</t>
-        </is>
-      </c>
+      <c r="I12" s="7" t="inlineStr"/>
       <c r="J12" s="7" t="inlineStr"/>
     </row>
-    <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B13" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D13" s="7" t="inlineStr"/>
-      <c r="E13" s="7" t="inlineStr"/>
-      <c r="F13" s="7" t="inlineStr"/>
-      <c r="G13" s="7" t="inlineStr"/>
-      <c r="H13" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="I13" s="7" t="inlineStr"/>
-      <c r="J13" s="7" t="inlineStr"/>
-    </row>
-    <row r="14"/>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A2:J2"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="25" customWidth="1" min="4" max="4"/>
-    <col width="25" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
-    <col width="25" customWidth="1" min="7" max="7"/>
-    <col width="25" customWidth="1" min="8" max="8"/>
-    <col width="25" customWidth="1" min="9" max="9"/>
-    <col width="25" customWidth="1" min="10" max="10"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>CANTHO UNIVERSITY SOFTWARE CENTER</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>TRUNG TÂM PHẦN MỀM ĐẠI HỌC CẦN THƠ</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>Khu 3, Đại học Cần Thơ - 01 Lý Tự Trọng, TP Cần Thơ - Tel: 0292.3731072 &amp; Fax: 0292.3731071 - Email: cusc@ctu.edu.vn</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>WEEK 7 TIMETABLE (22/09/2025 - 28/09/2025)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="40" customHeight="1">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>Time Slot</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>Class</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>Students</t>
-        </is>
-      </c>
-      <c r="D7" s="5" t="inlineStr">
-        <is>
-          <t>Monday
-22/09</t>
-        </is>
-      </c>
-      <c r="E7" s="5" t="inlineStr">
-        <is>
-          <t>Tuesday
-23/09</t>
-        </is>
-      </c>
-      <c r="F7" s="5" t="inlineStr">
-        <is>
-          <t>Wednesday
-24/09</t>
-        </is>
-      </c>
-      <c r="G7" s="5" t="inlineStr">
-        <is>
-          <t>Thursday
-25/09</t>
-        </is>
-      </c>
-      <c r="H7" s="5" t="inlineStr">
-        <is>
-          <t>Friday
-26/09</t>
-        </is>
-      </c>
-      <c r="I7" s="5" t="inlineStr">
-        <is>
-          <t>Saturday
-27/09</t>
-        </is>
-      </c>
-      <c r="J7" s="5" t="inlineStr">
-        <is>
-          <t>Sunday
-28/09</t>
-        </is>
-      </c>
-    </row>
-    <row r="8" ht="60" customHeight="1">
-      <c r="A8" s="6" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="B8" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C8" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>MH001
-(Theory)
-Room: LT3
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="7" t="inlineStr"/>
-      <c r="J8" s="7" t="inlineStr"/>
-    </row>
-    <row r="9" ht="60" customHeight="1">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>C2</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D9" s="7" t="inlineStr"/>
-      <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="9" t="inlineStr">
-        <is>
-          <t>MH001
-(Practice)
-Room: TH3
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH015
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
-        </is>
-      </c>
-      <c r="J9" s="7" t="inlineStr"/>
-    </row>
-    <row r="10" ht="60" customHeight="1">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="9" t="inlineStr">
-        <is>
-          <t>MH002
-(Practice)
-Room: TH3
-Lecturer: GV008</t>
-        </is>
-      </c>
-      <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="7" t="inlineStr"/>
-      <c r="I10" s="7" t="inlineStr"/>
-      <c r="J10" s="7" t="inlineStr"/>
-    </row>
-    <row r="11" ht="60" customHeight="1">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>MH009
-(Practice)
-Room: TH3
-Lecturer: GV003</t>
-        </is>
-      </c>
-      <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="7" t="inlineStr"/>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH016
-(Theory)
-Room: LT2
-Lecturer: GV006</t>
-        </is>
-      </c>
-      <c r="I11" s="7" t="inlineStr"/>
-      <c r="J11" s="7" t="inlineStr"/>
-    </row>
-    <row r="12" ht="60" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>T1</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="8" t="inlineStr">
-        <is>
-          <t>MH009
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
-      <c r="F12" s="7" t="inlineStr"/>
-      <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
-Lecturer: GV008</t>
-        </is>
-      </c>
-      <c r="I12" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT1
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="J12" s="7" t="inlineStr"/>
-    </row>
-    <row r="13" ht="60" customHeight="1">
-      <c r="A13" s="6" t="inlineStr">
-        <is>
-          <t>T2</t>
-        </is>
-      </c>
-      <c r="B13" s="7" t="inlineStr">
-        <is>
-          <t>DH23AI</t>
-        </is>
-      </c>
-      <c r="C13" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="D13" s="7" t="inlineStr"/>
-      <c r="E13" s="7" t="inlineStr"/>
-      <c r="F13" s="7" t="inlineStr"/>
-      <c r="G13" s="7" t="inlineStr"/>
-      <c r="H13" s="7" t="inlineStr"/>
-      <c r="I13" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT3
-Lecturer: GV008</t>
-        </is>
-      </c>
-      <c r="J13" s="7" t="inlineStr"/>
-    </row>
-    <row r="14"/>
+    <row r="13"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>
@@ -4488,24 +4465,45 @@
         <v>30</v>
       </c>
       <c r="D8" s="7" t="inlineStr"/>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>MH001
+      <c r="E8" s="9" t="inlineStr">
+        <is>
+          <t>MH002
 (Theory)
 Room: LT3
 Lecturer: GV001</t>
         </is>
       </c>
+      <c r="F8" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
+        </is>
+      </c>
+      <c r="G8" s="9" t="inlineStr">
+        <is>
+          <t>MH001
+(Theory)
+Room: A101
+Lecturer: GV001</t>
+        </is>
+      </c>
       <c r="H8" s="7" t="inlineStr"/>
-      <c r="I8" s="7" t="inlineStr"/>
+      <c r="I8" s="8" t="inlineStr">
+        <is>
+          <t>MH002
+(Practice)
+Room: TH1
+Lecturer: GV008</t>
+        </is>
+      </c>
       <c r="J8" s="7" t="inlineStr"/>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -4518,22 +4516,22 @@
       </c>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="9" t="inlineStr">
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="7" t="inlineStr"/>
+      <c r="H9" s="8" t="inlineStr">
         <is>
           <t>MH001
 (Practice)
-Room: TH3
+Room: TH1
 Lecturer: GV001</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH015
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
+      <c r="I9" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
         </is>
       </c>
       <c r="J9" s="7" t="inlineStr"/>
@@ -4541,7 +4539,7 @@
     <row r="10" ht="60" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
@@ -4553,31 +4551,24 @@
         <v>30</v>
       </c>
       <c r="D10" s="7" t="inlineStr"/>
-      <c r="E10" s="9" t="inlineStr">
-        <is>
-          <t>MH002
-(Practice)
-Room: TH3
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="9" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: A102
 Lecturer: GV008</t>
         </is>
       </c>
-      <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT1
-Lecturer: GV008</t>
-        </is>
-      </c>
+      <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
     <row r="11" ht="60" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>T1</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
@@ -4588,39 +4579,25 @@
       <c r="C11" s="7" t="n">
         <v>30</v>
       </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>MH009
-(Practice)
-Room: TH3
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
       <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH016
-(Theory)
-Room: LT2
-Lecturer: GV006</t>
-        </is>
-      </c>
-      <c r="I11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
-Lecturer: GV008</t>
-        </is>
-      </c>
+      <c r="H11" s="9" t="inlineStr">
+        <is>
+          <t>MH012
+(Theory)
+Room: LT1
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
       <c r="J11" s="7" t="inlineStr"/>
     </row>
     <row r="12" ht="60" customHeight="1">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>T2</t>
         </is>
       </c>
       <c r="B12" s="7" t="inlineStr">
@@ -4632,32 +4609,18 @@
         <v>30</v>
       </c>
       <c r="D12" s="7" t="inlineStr"/>
-      <c r="E12" s="8" t="inlineStr">
-        <is>
-          <t>MH009
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="E12" s="7" t="inlineStr"/>
       <c r="F12" s="7" t="inlineStr"/>
       <c r="G12" s="7" t="inlineStr"/>
-      <c r="H12" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT1
 Lecturer: GV008</t>
         </is>
       </c>
-      <c r="I12" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT1
-Lecturer: GV001</t>
-        </is>
-      </c>
+      <c r="I12" s="7" t="inlineStr"/>
       <c r="J12" s="7" t="inlineStr"/>
     </row>
     <row r="13"/>
@@ -4678,7 +4641,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4802,11 +4765,11 @@
       <c r="D8" s="7" t="inlineStr"/>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
+      <c r="G8" s="9" t="inlineStr">
         <is>
           <t>MH001
 (Theory)
-Room: LT3
+Room: A101
 Lecturer: GV001</t>
         </is>
       </c>
@@ -4817,7 +4780,7 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -4833,12 +4796,12 @@
       <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="8" t="inlineStr">
-        <is>
-          <t>MH015
-(Theory)
-Room: LT3
-Lecturer: GV002</t>
+      <c r="I9" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT4
+Lecturer: GV001</t>
         </is>
       </c>
       <c r="J9" s="7" t="inlineStr"/>
@@ -4860,15 +4823,15 @@
       <c r="D10" s="7" t="inlineStr"/>
       <c r="E10" s="7" t="inlineStr"/>
       <c r="F10" s="7" t="inlineStr"/>
-      <c r="G10" s="7" t="inlineStr"/>
-      <c r="H10" s="8" t="inlineStr">
-        <is>
-          <t>MH016
-(Theory)
-Room: LT2
-Lecturer: GV006</t>
-        </is>
-      </c>
+      <c r="G10" s="9" t="inlineStr">
+        <is>
+          <t>MH013
+(Theory)
+Room: A102
+Lecturer: GV008</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
       <c r="I10" s="7" t="inlineStr"/>
       <c r="J10" s="7" t="inlineStr"/>
     </row>
@@ -4887,35 +4850,50 @@
         <v>30</v>
       </c>
       <c r="D11" s="7" t="inlineStr"/>
-      <c r="E11" s="8" t="inlineStr">
-        <is>
-          <t>MH009
-(Theory)
-Room: LT1
-Lecturer: GV003</t>
-        </is>
-      </c>
+      <c r="E11" s="7" t="inlineStr"/>
       <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT4
+      <c r="H11" s="9" t="inlineStr">
+        <is>
+          <t>MH012
+(Theory)
+Room: LT1
+Lecturer: GV005</t>
+        </is>
+      </c>
+      <c r="I11" s="7" t="inlineStr"/>
+      <c r="J11" s="7" t="inlineStr"/>
+    </row>
+    <row r="12" ht="60" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>T2</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>DH23AI</t>
+        </is>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="inlineStr"/>
+      <c r="E12" s="7" t="inlineStr"/>
+      <c r="F12" s="7" t="inlineStr"/>
+      <c r="G12" s="7" t="inlineStr"/>
+      <c r="H12" s="9" t="inlineStr">
+        <is>
+          <t>MH002
+(Theory)
+Room: LT1
 Lecturer: GV008</t>
         </is>
       </c>
-      <c r="I11" s="8" t="inlineStr">
-        <is>
-          <t>MH002
-(Theory)
-Room: LT1
-Lecturer: GV001</t>
-        </is>
-      </c>
-      <c r="J11" s="7" t="inlineStr"/>
-    </row>
-    <row r="12"/>
+      <c r="I12" s="7" t="inlineStr"/>
+      <c r="J12" s="7" t="inlineStr"/>
+    </row>
+    <row r="13"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:J1"/>

</xml_diff>